<commit_message>
Add the first iteration of the randomizer
</commit_message>
<xml_diff>
--- a/Player Mats.xlsx
+++ b/Player Mats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C197DD6-FCF6-412F-9A96-71738C16B5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08BE971-49E6-441C-91A5-9AB0C9C0B9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{200934F6-D022-405E-A714-D004743EF374}"/>
   </bookViews>
@@ -1133,21 +1133,9 @@
     <t>Every mage in Azer has a Tether, right? That super special partner who they fight with and protect more than anyone else? The center of their universe? How special for them. I don't need that. Never have, never will, and I'm sick of everyone treating me like I'm fragile and damage just because I'm on my own. I liked being on my own. I'm strong like this. Who needs to channel aether when you can simply tear open a conduit and let the power overwhelm you? The teachers says I'm reckless. I say I get results. I used to have a Tether, way back when. If I focus really hard, I can even remember his face. Green hair. Pale eyes. He had a weird penchant for plants and a tendency to wander off into the woods for hours at a time. One day he wandered off and simply didn't come back. We hadn't even had our tattoos done yet. What was I supposed to do? A single mage abandoned by her Tether and left to create my own kind of magic. So I did. A magic more powerful because I didn't have some partner holding me back. I don't need guidelines, I don't need a Tether, and I definitely don't need anyone's help.</t>
   </si>
   <si>
-    <t>Own Mage 1 (Bow)</t>
-  </si>
-  <si>
     <t>Legacy</t>
   </si>
   <si>
-    <t>Own Mage 2 (Sword)</t>
-  </si>
-  <si>
-    <t>Own Mage 3 (Ram)</t>
-  </si>
-  <si>
-    <t>Own Mage 4 (Staff)</t>
-  </si>
-  <si>
     <t>0,2,4,3</t>
   </si>
   <si>
@@ -1227,6 +1215,18 @@
   </si>
   <si>
     <t>0,1,1,1</t>
+  </si>
+  <si>
+    <t>Legacy Mage 1 (Bow)</t>
+  </si>
+  <si>
+    <t>Legacy Mage 2 (Sword)</t>
+  </si>
+  <si>
+    <t>Legacy Mage 3 (Ram)</t>
+  </si>
+  <si>
+    <t>Legacy Mage 4 (Staff)</t>
   </si>
 </sst>
 </file>
@@ -1687,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78882F6F-0A17-4313-838D-7610DDA9696E}">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1846,7 +1846,7 @@
         <v>72</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>23</v>
@@ -1902,7 +1902,7 @@
         <v>72</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>32</v>
@@ -1958,7 +1958,7 @@
         <v>72</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>40</v>
@@ -2014,7 +2014,7 @@
         <v>72</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>46</v>
@@ -2070,7 +2070,7 @@
         <v>72</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>52</v>
@@ -2126,7 +2126,7 @@
         <v>72</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>58</v>
@@ -2182,7 +2182,7 @@
         <v>72</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>64</v>
@@ -2238,7 +2238,7 @@
         <v>72</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>70</v>
@@ -2294,7 +2294,7 @@
         <v>72</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>79</v>
@@ -2350,7 +2350,7 @@
         <v>72</v>
       </c>
       <c r="J12" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>32</v>
@@ -2406,7 +2406,7 @@
         <v>72</v>
       </c>
       <c r="J13" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>91</v>
@@ -2462,7 +2462,7 @@
         <v>72</v>
       </c>
       <c r="J14" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>79</v>
@@ -2565,7 +2565,7 @@
         <v>72</v>
       </c>
       <c r="J16" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>103</v>
@@ -2621,7 +2621,7 @@
         <v>72</v>
       </c>
       <c r="J17" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>110</v>
@@ -2677,7 +2677,7 @@
         <v>72</v>
       </c>
       <c r="J18" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>116</v>
@@ -2733,7 +2733,7 @@
         <v>72</v>
       </c>
       <c r="J19" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>123</v>
@@ -2789,7 +2789,7 @@
         <v>72</v>
       </c>
       <c r="J20" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>58</v>
@@ -2845,7 +2845,7 @@
         <v>72</v>
       </c>
       <c r="J21" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>64</v>
@@ -2901,7 +2901,7 @@
         <v>72</v>
       </c>
       <c r="J22" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>70</v>
@@ -2957,7 +2957,7 @@
         <v>72</v>
       </c>
       <c r="J23" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>144</v>
@@ -3013,7 +3013,7 @@
         <v>72</v>
       </c>
       <c r="J24" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>79</v>
@@ -3069,7 +3069,7 @@
         <v>72</v>
       </c>
       <c r="J25" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>32</v>
@@ -3125,7 +3125,7 @@
         <v>72</v>
       </c>
       <c r="J26" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>161</v>
@@ -3181,7 +3181,7 @@
         <v>72</v>
       </c>
       <c r="J27" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>91</v>
@@ -3284,7 +3284,7 @@
         <v>72</v>
       </c>
       <c r="J29" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>176</v>
@@ -3340,7 +3340,7 @@
         <v>72</v>
       </c>
       <c r="J30" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>184</v>
@@ -3396,7 +3396,7 @@
         <v>72</v>
       </c>
       <c r="J31" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>192</v>
@@ -3452,7 +3452,7 @@
         <v>72</v>
       </c>
       <c r="J32" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>200</v>
@@ -3508,7 +3508,7 @@
         <v>72</v>
       </c>
       <c r="J33" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>206</v>
@@ -3564,7 +3564,7 @@
         <v>212</v>
       </c>
       <c r="J34" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>213</v>
@@ -3620,7 +3620,7 @@
         <v>72</v>
       </c>
       <c r="J35" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>220</v>
@@ -3676,7 +3676,7 @@
         <v>227</v>
       </c>
       <c r="J36" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>228</v>
@@ -3732,7 +3732,7 @@
         <v>234</v>
       </c>
       <c r="J37" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>235</v>
@@ -3788,7 +3788,7 @@
         <v>244</v>
       </c>
       <c r="J38" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>245</v>
@@ -3844,7 +3844,7 @@
         <v>72</v>
       </c>
       <c r="J39" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>235</v>
@@ -3900,7 +3900,7 @@
         <v>258</v>
       </c>
       <c r="J40" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>117</v>
@@ -3956,7 +3956,7 @@
         <v>266</v>
       </c>
       <c r="J41" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>267</v>
@@ -4059,7 +4059,7 @@
         <v>72</v>
       </c>
       <c r="J43" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>274</v>
@@ -4115,7 +4115,7 @@
         <v>72</v>
       </c>
       <c r="J44" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>282</v>
@@ -4171,7 +4171,7 @@
         <v>289</v>
       </c>
       <c r="J45" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>290</v>
@@ -4227,7 +4227,7 @@
         <v>296</v>
       </c>
       <c r="J46" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>200</v>
@@ -4283,7 +4283,7 @@
         <v>72</v>
       </c>
       <c r="J47" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>304</v>
@@ -4339,7 +4339,7 @@
         <v>72</v>
       </c>
       <c r="J48" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>310</v>
@@ -4395,7 +4395,7 @@
         <v>320</v>
       </c>
       <c r="J49" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>321</v>
@@ -4451,7 +4451,7 @@
         <v>72</v>
       </c>
       <c r="J50" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>328</v>
@@ -4507,7 +4507,7 @@
         <v>334</v>
       </c>
       <c r="J51" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>335</v>
@@ -4563,7 +4563,7 @@
         <v>342</v>
       </c>
       <c r="J52" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>343</v>
@@ -4619,7 +4619,7 @@
         <v>72</v>
       </c>
       <c r="J53" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>352</v>
@@ -4675,7 +4675,7 @@
         <v>72</v>
       </c>
       <c r="J54" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>362</v>
@@ -4721,7 +4721,7 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>365</v>
+        <v>393</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>72</v>
@@ -4766,12 +4766,12 @@
         <v>72</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>367</v>
+        <v>394</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>72</v>
@@ -4816,12 +4816,12 @@
         <v>72</v>
       </c>
       <c r="R57" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>368</v>
+        <v>395</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>72</v>
@@ -4866,12 +4866,12 @@
         <v>72</v>
       </c>
       <c r="R58" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>369</v>
+        <v>396</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>72</v>
@@ -4916,7 +4916,7 @@
         <v>72</v>
       </c>
       <c r="R59" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prepare mages for the upcoming Legacy of Gravehold
</commit_message>
<xml_diff>
--- a/Player Mats.xlsx
+++ b/Player Mats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Lexive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08BE971-49E6-441C-91A5-9AB0C9C0B9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA5461C-A4DF-494A-ABA2-8F80433A40B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{200934F6-D022-405E-A714-D004743EF374}"/>
   </bookViews>
@@ -143,9 +143,6 @@
     <t>My conclave of sisters is long ago gone, all of them ash in the world above. I do not remember their names, only their faces and the brightness in their eyes. Their songs fade in the gray shadows of my many years, and I alone can still hear them. Only Gravehold is more ancient than I. Yet somehow I endure.#This city looks to me for guidance, for I have walked a long, wearisome path to stand before them. This is my duty, my burden, my privilege. It was I who counseled them to collapse the mouth of the cave, to entomb us here. It was I who taught the mages to wield the sister-words. Where so many have slipped beneath the shadow, I have remained in light.#Many say we are lost, that Gravehold is just that: our grave. They say that, like my sisters, we will be erased, our bones left to molder in the silence of this cave. But glory will be ours again and I will live to feel the sun and wind on my face once more. Faith, younglings. It is our best weapon.</t>
   </si>
   <si>
-    <t>Kadir</t>
-  </si>
-  <si>
     <t>Breach Mage Delver</t>
   </si>
   <si>
@@ -317,9 +314,6 @@
     <t>I lost the arm to tainted jade. I felt it creeping through my arteries and lopped it off without a thought. Best to lose the arm and keep the rest, no?#Kadir says I was born for this, meant to live here and now in this damnable hole in the ground to fight these things. And she has the right of it. This is who I am, what I am: a blunt instrument to be used against monsters. My life matters not for much more than that. And I am at peace with it.#Whenever those bells ring I feel my heart swell as I heave my chopper from its sheath. I smell the air burn as the breach opens and I cannot run there fast enough. We all have a purpose, a gift to give. This is mine.</t>
   </si>
   <si>
-    <t>Malastar</t>
-  </si>
-  <si>
     <t>Breach Mage Mentor</t>
   </si>
   <si>
@@ -395,9 +389,6 @@
     <t>"One. Two. Three. Four. Five.#One. In the monastery cavern, when I was but a child. The morning I earned some of these scars. So far away, back in The World That Was. The monks found me first, bleeding and blasted. When they asked what had happened, I said only that I killed it. What else needed to be said? They didn't believe me until they found its body under the ruined wall. The monks started training me the very next day.#Two. At the end of my training. A test of my skills. The monks suggested a lesser being, but I wanted to bring back one of my own choosing, one that would move me further on the path. I dragged its head behind me for days before I found my way back. I graduated late, but with the highest distinction.#Three. I lay in wait for this one. It had to be this one, for the path, and this place was the only place where one of these beasts had ever been seen. I lay in wait a long time. By the end of the third year, I began to despair of its existence. My patience was rewarded. The greatest lesson an assassin learns is not how to kill. It's how to wait.#Four and five are yet to come. But I know they will come to me and offer themselves through combat. And I will kill them and move along the path. Each step brings me closer. Each kill brings me closer to the mind of the gods. Look into the eyes when you make a kill. You may get a glimpse of the creature's true master."</t>
   </si>
   <si>
-    <t>Yan Magda</t>
-  </si>
-  <si>
     <t>Enlightened Exile</t>
   </si>
   <si>
@@ -509,9 +500,6 @@
     <t>"What I'm saying is, we're making it too complicated. Ever since they showed up, it's been bicker and argue, argue and bicker. Why all this talk? We know we need to fight, so let's go fight. No talking needed for talk.#Brama says Yan and her pack of miscreants are heretics and cannot be trusted, that the help they gave in the battle with the Thrice-Dead Prophet was just to throw us off. I bet they saw we were winning anyway; we could have done it without them no matter what anybody says. And let us not forget the aftermath of that fight...#I have an idea -- keep them fighting The Nameless. They will die in battle, or they'll slip up and betray their true loyalty, in which case I'll kill them myself. Either way we'll be rid of them, and that suits me just fine."</t>
   </si>
   <si>
-    <t>Indira</t>
-  </si>
-  <si>
     <t>Breach Apprentice</t>
   </si>
   <si>
@@ -578,9 +566,6 @@
     <t>The New Age</t>
   </si>
   <si>
-    <t>Gygar</t>
-  </si>
-  <si>
     <t>Tide Master</t>
   </si>
   <si>
@@ -623,9 +608,6 @@
     <t>Danger unifies. Tragedy hardens. Desperation brings out the deepest strength in a person's soul. This is why the people of Gravehold cling like cockroaches to the surface of this world that hates us. I was a child when my mother, Z'hana, pulled me sobbing out of the collapsing tunnels. My father was in too deep, fighting to protect us against Maelstrom. I watched, helpless, as he vanished behind the rocks. I will always remember listening to my mother, the strongest person I know, crying herself to sleep. The next morning she sat me down and brushed the hair from my eyes. She said, "I want to see you grow up in peace, my child, but our world does not know peace. I wish you could grow up feeling safe, but this city is not safe. Your father and I have tried to give you a better future, but we failed. I'm sorry, my love. All I can give you now is the strength to keep fighting. Succeed where we could not. Make this world a place where your children do not need to struggle to survive. Become strong, but do not become a weapon. Become their shield."</t>
   </si>
   <si>
-    <t>Claudia</t>
-  </si>
-  <si>
     <t>Prospector</t>
   </si>
   <si>
@@ -662,9 +644,6 @@
     <t>When I was a kid I started losing my hair. No one knew what was happening, not even Brama. I was weak, bedridden for months. My folks figured I was gonna die, they cried over me while I drifted in and outta consciousness. They talked like I was already gone, sayin' how I'd be at peace now and all. Screw that. I've never been at peace my whole life. This whole world has never been at peace. Life is a battle and I'm not the givin' up type. Don't ask me how I found the strength but one night I got outta bed and stumbled into my dad's laboratory. I grabbed hold of one of the artifacts he'd been researching and poured every scrap of magical energy I had into it. I felt my skin changing and a tingle on my scalp. My hair began to grow back, strange and crystalline. Somehow, that infusion of breach magic fixed me. Brama has never stopped trying to find the secret to my healing. No one knows why I got sick or how I got better, or where my new hair comes from, but I don't care. Every day I walk on my own two feet is a day I stole from the Void. And I'm not done fighting yet.</t>
   </si>
   <si>
-    <t>Soskel</t>
-  </si>
-  <si>
     <t>Aristocrat</t>
   </si>
   <si>
@@ -686,9 +665,6 @@
     <t>It wasn't until Arachnos captured me and forced Void essence into my very soul that I understood what true power is. It's the potential to make a difference, to save those you love. My whole life I've only wanted to serve and protect Gravehold but I was never strong enough. It's my home, and its people are my family. As a youth, I carried crying children as we ran from The Fall, told them stories to help them sleep as we wandered the tunnels. I was a nobody, but I wanted to be useful. I had to defend what was left. After that day, I vowed to never again be so helpless. I needed to understand breach magic, but Mist said it was uncommon for an adult to become a mage initiate. I watched the children I had saved surpass me, become prodigious mages and burn brighter than I ever imagined. When Brama selected me as commander of an expedition to the north, I was shocked. My breach magic was certainly competent, but I was nowhere near as powerful as the mages she put under my leadership. I asked her why she chose me and Brama smiled. She said that while power is important, the true mark of a leader is understanding those he leads. It was this discipline, and my familiarity with loss, that let me survive the torture of Arachnos' ritual without forgetting myself. I have watched friends die too many times. This power may be corrupted, but if I can use it to help, I won't hold back.</t>
   </si>
   <si>
-    <t>Talix</t>
-  </si>
-  <si>
     <t>The Chain</t>
   </si>
   <si>
@@ -707,9 +683,6 @@
     <t>It was kind of lonely growing up in Southpost. There weren't many kids my age to play with so I made my own fun by exploring the wilds. It was against the rules to go out alone, but that was what made it so fun. As the top dog of Southpost, my mom had more important things to do than keep a super close eye on me. So I spent a lot of time at home. Studying. Right next to a conveniently unlocked window. I knew it was stupid to wander around alone, but I was a kid. Kids are stupid. And I was still an idiot well into my adulthood. I never saw the point of growing up until I had a kid of my own. I found him, Inco, in some ancient ruins, curled up for warmth and half buried in vines that I later learned were part of him. I'm still amazed by how much power he holds in that tiny body of his. I suppose he'd have to be strong, growing up out in the wilds. It's crazy, I was the first other human he ever met in his whole life. It took a while to get him to trust me, but finally I convinced him to come back to Southpost with me. After a few months we moved to New Gravehold together so Inco could be around kids his own age. I know what it's like to feel alone, isolated from your people. As long as I'm here, Inco will never feel that way.</t>
   </si>
   <si>
-    <t>Lost</t>
-  </si>
-  <si>
     <t>Living Forge</t>
   </si>
   <si>
@@ -728,9 +701,6 @@
     <t>"After we defeated that massive wolf-like Nameless, we found this suit of armor hiding below ground. Lost managed to remember that he was a mage of Gravehold, but we don't know which mage, nor how he found himself bound to this suit of armor. During The Fall, the tunnels collapsed, which sealed off outposts and scouting parties. We never learned the fate of many breach mages during that time. Already some people treat Lost like a ghost returned from our unhappy past. Some, myself included, can't help but see him as a sign that all our missing friends might still be out there. I know it's foolish to get caught up in baseless hopes, but I still want to believe we could find just one more mage. After all, who knows how long Lost has been down there, waiting patiently for someone to come. Not knowing who he is, forging weapons he didn't know how to use. But I am hopeful. Each day, Lost's connection to us all grows stronger. Perhaps we may one day be able to reunite him with loved ones." - Soskel</t>
   </si>
   <si>
-    <t>Mazra</t>
-  </si>
-  <si>
     <t>The Reader</t>
   </si>
   <si>
@@ -782,9 +752,6 @@
     <t>Even though he was my father, I never really knew Xaxos. Not like some of his old friends here in Gravehold. Growing up, I could tell I was looking at the shell of a man. I was seeing someone desperately trying to piece himself back together, to regain something lost, to return to the man he was before. I never met the man my father was. The Void changes people. I should know, I lived my whole life there. I wonder, now, if the Nameless fight and kill because the very essence of their world drives them to it. Bloodlust permeates the air, twisting their minds. Or perhaps it is the emptiness, the barren nothing they are born into forces them into action. Growing up here, I understand what drives them towards the portals. The first time I saw a breach open I dropped everything. I didn't stop to think about my father, his research, our home, or my things. Everything paled in comparison to the potential to escape. I doubt he will ever even notice I am gone. Time is warped, it passes differently inside the Void. I don't know how old I am, or how long I have been gone, or where my place is in this strange world. But I know New Gravehold is beautiful. Humans are beautiful. Perhaps it is because of my humanity that I can control the Void energy that has consumed me my entire life. I've embraced my rage, channeled my hurt, and funneled my passion outward into strength. I will not let the Nameless have this world too, not when I have only just found it.</t>
   </si>
   <si>
-    <t>Nook</t>
-  </si>
-  <si>
     <t>Orb Caller</t>
   </si>
   <si>
@@ -800,9 +767,6 @@
     <t>Shattered Dreams</t>
   </si>
   <si>
-    <t>Inco</t>
-  </si>
-  <si>
     <t>Child of Green</t>
   </si>
   <si>
@@ -824,9 +788,6 @@
     <t>Into the Wild</t>
   </si>
   <si>
-    <t>Razra</t>
-  </si>
-  <si>
     <t>The Trainer</t>
   </si>
   <si>
@@ -848,9 +809,6 @@
     <t>"Razra and I may be identical but we couldn't be more different. She's always taken the fact that we live in a jungle full of deadly monsters as more of a challenge than something to fear. She was the sort of child who would break her leg jumping off the roof, and before it even healed, jump off again because now she's sure she's perfected the landing. I think these days the dirt might be so deeply ingrained in her skin that it won't ever come off. It's no wonder she's so close with that strange forest boy, Inco. I'll admit, I worried about her for a long time. We had both always wanted to become breach mages. While it came naturally to me, Razra struggled. She wouldn't focus on a book, couldn't sit through a lesson. Then, as if it was sent for her, that strange creature wandered close to the city. No normal person would even care, but my sister has never been normal. She threw herself into befriending this creature, named it Rip, and trained it beyond what anyone had assumed possible. It was miraculous. With Rip by her side Razra grew quickly in strength, racing through her training at unprecedented speeds. Finally, she joined me as a full fledged breach mage. I was starting to get bored waiting for her to catch up." - Mazra</t>
   </si>
   <si>
-    <t>Ilya</t>
-  </si>
-  <si>
     <t>Right Hand</t>
   </si>
   <si>
@@ -872,9 +830,6 @@
     <t>Outcasts</t>
   </si>
   <si>
-    <t>Kel</t>
-  </si>
-  <si>
     <t>Left Hand</t>
   </si>
   <si>
@@ -956,9 +911,6 @@
     <t>I spent so much of my life desperate to escape the Void, it's odd to find myself returned. My new life in New Gravehold is so beautiful that I am almost afraid to touch it, as if it might shatter like brittle glass. I have people I would consider friends. I have a house that I am trying to consider a home. Taqren tells me it's normal to be nostalgic for a battleground. He says he too has dreams of the fearful weeks he spent running from Gravehold as the caves collapsed, hunted by Nameless with almost no protection. At least then he had purpose, clarity of direction. Now my bed is so comfortable, I don't feel like I belong in it. The people are so carefully kind, they avoid my monstrous half with practiced courtesy, and I know they are not ready. So I was almost relieved to follow my father's call and return to this dreaded place where everything is pain and fear and suffering, but it is at least a familiar pain. I know the shape of this pain, where it inserts itself beneath my ribs and settles. It does not try to hide behind honeyed words. I do not want to stay here, in this dark place. But maybe by the time I have returned, New Gravehold will be ready for me. Maybe I will finally be ready for it.</t>
   </si>
   <si>
-    <t>Thraxir</t>
-  </si>
-  <si>
     <t>Reanimated</t>
   </si>
   <si>
@@ -1227,6 +1179,54 @@
   </si>
   <si>
     <t>Legacy Mage 4 (Staff)</t>
+  </si>
+  <si>
+    <t>Kadir (AE)</t>
+  </si>
+  <si>
+    <t>Malastar (AE)</t>
+  </si>
+  <si>
+    <t>Yan Magda (WE)</t>
+  </si>
+  <si>
+    <t>Indira (WE)</t>
+  </si>
+  <si>
+    <t>Gygar (NA)</t>
+  </si>
+  <si>
+    <t>Claudia (NA)</t>
+  </si>
+  <si>
+    <t>Soskel (NA)</t>
+  </si>
+  <si>
+    <t>Talix (NA)</t>
+  </si>
+  <si>
+    <t>Lost (NA)</t>
+  </si>
+  <si>
+    <t>Mazra (NA)</t>
+  </si>
+  <si>
+    <t>Nook (NA)</t>
+  </si>
+  <si>
+    <t>Inco (NA)</t>
+  </si>
+  <si>
+    <t>Razra (NA)</t>
+  </si>
+  <si>
+    <t>Ilya (O)</t>
+  </si>
+  <si>
+    <t>Kel (O)</t>
+  </si>
+  <si>
+    <t>Thraxir (O)</t>
   </si>
 </sst>
 </file>
@@ -1687,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78882F6F-0A17-4313-838D-7610DDA9696E}">
   <dimension ref="A1:R59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,52 +1769,52 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1837,16 +1837,16 @@
         <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>23</v>
@@ -1855,16 +1855,16 @@
         <v>24</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>25</v>
@@ -1893,16 +1893,16 @@
         <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>32</v>
@@ -1911,16 +1911,16 @@
         <v>33</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>34</v>
@@ -1931,55 +1931,55 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1">
         <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>26</v>
@@ -1987,55 +1987,55 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="1">
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>26</v>
@@ -2043,16 +2043,16 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
@@ -2061,37 +2061,37 @@
         <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>26</v>
@@ -2099,16 +2099,16 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="1">
         <v>4</v>
@@ -2117,37 +2117,37 @@
         <v>30</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>26</v>
@@ -2155,55 +2155,55 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C9" s="1">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="1">
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>26</v>
@@ -2211,55 +2211,55 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C10" s="1">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="1">
         <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>26</v>
@@ -2267,16 +2267,16 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C11" s="1">
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E11" s="1">
         <v>5</v>
@@ -2285,54 +2285,54 @@
         <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E12">
         <v>6</v>
@@ -2341,54 +2341,54 @@
         <v>30</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J12" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="C13">
         <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -2397,54 +2397,54 @@
         <v>30</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J13" t="s">
+        <v>352</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J13" t="s">
-        <v>368</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>93</v>
+        <v>382</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C14">
         <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E14">
         <v>6</v>
@@ -2453,101 +2453,101 @@
         <v>30</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J14" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C16">
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E16">
         <v>6</v>
@@ -2556,54 +2556,54 @@
         <v>30</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J16" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C17">
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E17">
         <v>6</v>
@@ -2612,54 +2612,54 @@
         <v>30</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J17" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -2668,54 +2668,54 @@
         <v>30</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J18" t="s">
+        <v>355</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J18" t="s">
-        <v>371</v>
-      </c>
-      <c r="K18" s="1" t="s">
+      <c r="M18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q18" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="L18" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="R18" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>119</v>
+        <v>383</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E19">
         <v>5</v>
@@ -2724,54 +2724,54 @@
         <v>30</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J19" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E20">
         <v>6</v>
@@ -2780,54 +2780,54 @@
         <v>30</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J20" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C21">
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E21">
         <v>5</v>
@@ -2836,54 +2836,54 @@
         <v>30</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J21" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E22">
         <v>5</v>
@@ -2892,54 +2892,54 @@
         <v>30</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J22" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C23">
         <v>5</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -2948,54 +2948,54 @@
         <v>30</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J23" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C24">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -3004,54 +3004,54 @@
         <v>30</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J24" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C25">
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E25">
         <v>5</v>
@@ -3060,16 +3060,16 @@
         <v>30</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J25" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>32</v>
@@ -3078,36 +3078,36 @@
         <v>24</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>157</v>
+        <v>384</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C26">
         <v>9</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -3116,54 +3116,54 @@
         <v>30</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H26" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J26" t="s">
+        <v>365</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="R26" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J26" t="s">
-        <v>381</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C27">
         <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E27">
         <v>5</v>
@@ -3172,157 +3172,157 @@
         <v>30</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J27" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C29">
         <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E29">
         <v>4</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J29" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>180</v>
+        <v>385</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -3331,54 +3331,54 @@
         <v>30</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J30" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E31">
         <v>4</v>
@@ -3387,110 +3387,110 @@
         <v>30</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J31" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>195</v>
+        <v>386</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C32">
         <v>5</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E32">
         <v>5</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J32" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C33">
         <v>6</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="E33">
         <v>4</v>
@@ -3499,54 +3499,54 @@
         <v>30</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J33" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>24</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>208</v>
+        <v>387</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="E34">
         <v>4</v>
@@ -3555,54 +3555,54 @@
         <v>30</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="J34" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>216</v>
+        <v>388</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C35">
         <v>6</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E35">
         <v>5</v>
@@ -3611,54 +3611,54 @@
         <v>30</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J35" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>223</v>
+        <v>389</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C36">
         <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E36">
         <v>5</v>
@@ -3667,54 +3667,54 @@
         <v>30</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="J36" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>230</v>
+        <v>390</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C37">
         <v>6</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="E37">
         <v>4</v>
@@ -3723,54 +3723,54 @@
         <v>30</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="J37" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C38">
         <v>8</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="E38">
         <v>5</v>
@@ -3779,54 +3779,54 @@
         <v>30</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="J38" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>248</v>
+        <v>391</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="C39">
         <v>9</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="E39">
         <v>5</v>
@@ -3835,54 +3835,54 @@
         <v>30</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J39" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>254</v>
+        <v>392</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="C40">
         <v>4</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="E40">
         <v>5</v>
@@ -3891,54 +3891,54 @@
         <v>30</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="J40" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>262</v>
+        <v>393</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C41">
         <v>7</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="E41">
         <v>4</v>
@@ -3947,101 +3947,101 @@
         <v>30</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="J41" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>270</v>
+        <v>394</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="C43">
         <v>4</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="E43">
         <v>5</v>
@@ -4050,54 +4050,54 @@
         <v>30</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J43" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>278</v>
+        <v>395</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="C44">
         <v>4</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="E44">
         <v>6</v>
@@ -4106,54 +4106,54 @@
         <v>30</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J44" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="C45">
         <v>6</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="E45">
         <v>5</v>
@@ -4162,166 +4162,166 @@
         <v>30</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="J45" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="R45" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C46">
         <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="E46">
         <v>5</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="J46" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="C47">
         <v>7</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="E47">
         <v>4</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J47" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>306</v>
+        <v>396</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="C48">
         <v>5</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="E48">
         <v>5</v>
@@ -4330,54 +4330,54 @@
         <v>30</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J48" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="R48" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="C49">
         <v>7</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="E49">
         <v>4</v>
@@ -4386,54 +4386,54 @@
         <v>30</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="J49" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="C50">
         <v>3</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="E50">
         <v>6</v>
@@ -4442,54 +4442,54 @@
         <v>30</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J50" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="R50" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="C51">
         <v>4</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="E51">
         <v>6</v>
@@ -4498,54 +4498,54 @@
         <v>30</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="J51" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q51" s="1" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="C52">
         <v>4</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="E52">
         <v>4</v>
@@ -4554,110 +4554,110 @@
         <v>30</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="J52" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="Q52" s="1" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="R52" s="1" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="C53">
         <v>7</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="E53">
         <v>5</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J53" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="P53" s="1" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="R53" s="1" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="C54">
         <v>5</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="E54">
         <v>5</v>
@@ -4666,40 +4666,40 @@
         <v>30</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J54" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>33</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="P54" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="R54" s="1" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -4721,202 +4721,202 @@
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C56">
         <v>3</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C57">
         <v>3</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R57" s="1" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58">
         <v>3</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R58" s="1" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C59">
         <v>3</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q59" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R59" s="1" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>